<commit_message>
Second commit of the Project
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dooby\eclipse-workspace\RestASSUREDAPI\APITestingFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1673E4-079A-4977-825F-2DB8D045EAA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AE7A64-5827-4EA0-A476-249433F88A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,18 +112,12 @@
     <t>ValidateCreateCustomerAPIwithInValidSecretKey</t>
   </si>
   <si>
-    <t>at1@zmail.com</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>deleteCustomer</t>
   </si>
   <si>
-    <t>cus_JQbkukxgeA0kJ3</t>
-  </si>
-  <si>
     <t>Raunak111</t>
   </si>
   <si>
@@ -133,13 +127,19 @@
     <t>imraan111</t>
   </si>
   <si>
-    <t>rao11@zmail.com</t>
-  </si>
-  <si>
-    <t>ahpr11@zmail.com</t>
-  </si>
-  <si>
-    <t>imr11@zmail.com</t>
+    <t>rao112@zmail.com</t>
+  </si>
+  <si>
+    <t>ahpr112@zmail.com</t>
+  </si>
+  <si>
+    <t>imr112@zmail.com</t>
+  </si>
+  <si>
+    <t>at12@zmail.com</t>
+  </si>
+  <si>
+    <t>cus_JQcHyOgx0NzdKA</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,10 +502,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -513,10 +513,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -524,10 +524,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -554,7 +554,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -562,17 +562,17 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Third commit of the Project
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dooby\eclipse-workspace\RestASSUREDAPI\APITestingFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AE7A64-5827-4EA0-A476-249433F88A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98A10F5-856F-4D98-BAB5-15C0B6E81D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>email</t>
   </si>
@@ -136,10 +136,13 @@
     <t>imr112@zmail.com</t>
   </si>
   <si>
-    <t>at12@zmail.com</t>
-  </si>
-  <si>
-    <t>cus_JQcHyOgx0NzdKA</t>
+    <t>cus_JQcOWxkfkURlhm</t>
+  </si>
+  <si>
+    <t>cus_JQcNaXiIYdviRe</t>
+  </si>
+  <si>
+    <t>at123@zmail.com</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +557,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -572,6 +575,11 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>